<commit_message>
functional up to markdup with bwa
</commit_message>
<xml_diff>
--- a/sample_sheet.xlsx
+++ b/sample_sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTIONS!!!" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="43">
   <si>
     <t xml:space="preserve">INSTRUCTIONS</t>
   </si>
@@ -102,49 +102,55 @@
     <t xml:space="preserve">path_to_reads_2</t>
   </si>
   <si>
+    <t xml:space="preserve">/work/users/c/a/cannecar/ndj_project/reads/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ndj_04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ndj_05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ndj_06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ndj_07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ndj_08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ndj_09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ndj_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ndj_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ndj_12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ndj_13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ndj_14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ndj_15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ndj_16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hetsub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">path_to_reads</t>
+  </si>
+  <si>
     <t xml:space="preserve">/home/cam/test/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ndj_04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ndj_05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ndj_06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ndj_07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ndj_08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ndj_09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ndj_10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ndj_11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ndj_12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ndj_13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ndj_14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ndj_15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ndj_16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">path_to_reads</t>
   </si>
 </sst>
 </file>
@@ -262,15 +268,15 @@
   </sheetPr>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="72.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="29.08"/>
   </cols>
   <sheetData>
@@ -574,16 +580,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.77"/>
@@ -615,11 +621,11 @@
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">CONCATENATE(E2, A2, "_1.fq.gz")</f>
-        <v>/home/cam/test/w1118_1.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/w1118_1.fq.gz</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">CONCATENATE(E2, A2, "_2.fq.gz")</f>
-        <v>/home/cam/test/w1118_2.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/w1118_2.fq.gz</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>14</v>
@@ -634,11 +640,11 @@
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">CONCATENATE(E3, A3, "_1.fq.gz")</f>
-        <v>/home/cam/test/oregonr_1.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/oregonr_1.fq.gz</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">CONCATENATE(E3, A3, "_2.fq.gz")</f>
-        <v>/home/cam/test/oregonr_2.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/oregonr_2.fq.gz</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>14</v>
@@ -653,11 +659,11 @@
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">CONCATENATE(E4, A4, "_1.fq.gz")</f>
-        <v>/home/cam/test/ndj_01_1.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_01_1.fq.gz</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">CONCATENATE(E4, A4, "_2.fq.gz")</f>
-        <v>/home/cam/test/ndj_01_2.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_01_2.fq.gz</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>18</v>
@@ -672,11 +678,11 @@
       </c>
       <c r="B5" s="0" t="str">
         <f aca="false">CONCATENATE(E5, A5, "_1.fq.gz")</f>
-        <v>/home/cam/test/ndj_02_1.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_02_1.fq.gz</v>
       </c>
       <c r="C5" s="0" t="str">
         <f aca="false">CONCATENATE(E5, A5, "_2.fq.gz")</f>
-        <v>/home/cam/test/ndj_02_2.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_02_2.fq.gz</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>18</v>
@@ -691,11 +697,11 @@
       </c>
       <c r="B6" s="0" t="str">
         <f aca="false">CONCATENATE(E6, A6, "_1.fq.gz")</f>
-        <v>/home/cam/test/ndj_03_1.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_03_1.fq.gz</v>
       </c>
       <c r="C6" s="0" t="str">
         <f aca="false">CONCATENATE(E6, A6, "_2.fq.gz")</f>
-        <v>/home/cam/test/ndj_03_2.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_03_2.fq.gz</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>18</v>
@@ -710,11 +716,11 @@
       </c>
       <c r="B7" s="0" t="str">
         <f aca="false">CONCATENATE(E7, A7, "_1.fq.gz")</f>
-        <v>/home/cam/test/ndj_04_1.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_04_1.fq.gz</v>
       </c>
       <c r="C7" s="0" t="str">
         <f aca="false">CONCATENATE(E7, A7, "_2.fq.gz")</f>
-        <v>/home/cam/test/ndj_04_2.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_04_2.fq.gz</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>18</v>
@@ -729,11 +735,11 @@
       </c>
       <c r="B8" s="0" t="str">
         <f aca="false">CONCATENATE(E8, A8, "_1.fq.gz")</f>
-        <v>/home/cam/test/ndj_05_1.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_05_1.fq.gz</v>
       </c>
       <c r="C8" s="0" t="str">
         <f aca="false">CONCATENATE(E8, A8, "_2.fq.gz")</f>
-        <v>/home/cam/test/ndj_05_2.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_05_2.fq.gz</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>18</v>
@@ -748,11 +754,11 @@
       </c>
       <c r="B9" s="0" t="str">
         <f aca="false">CONCATENATE(E9, A9, "_1.fq.gz")</f>
-        <v>/home/cam/test/ndj_06_1.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_06_1.fq.gz</v>
       </c>
       <c r="C9" s="0" t="str">
         <f aca="false">CONCATENATE(E9, A9, "_2.fq.gz")</f>
-        <v>/home/cam/test/ndj_06_2.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_06_2.fq.gz</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>18</v>
@@ -767,11 +773,11 @@
       </c>
       <c r="B10" s="0" t="str">
         <f aca="false">CONCATENATE(E10, A10, "_1.fq.gz")</f>
-        <v>/home/cam/test/ndj_07_1.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_07_1.fq.gz</v>
       </c>
       <c r="C10" s="0" t="str">
         <f aca="false">CONCATENATE(E10, A10, "_2.fq.gz")</f>
-        <v>/home/cam/test/ndj_07_2.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_07_2.fq.gz</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>18</v>
@@ -786,11 +792,11 @@
       </c>
       <c r="B11" s="0" t="str">
         <f aca="false">CONCATENATE(E11, A11, "_1.fq.gz")</f>
-        <v>/home/cam/test/ndj_08_1.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_08_1.fq.gz</v>
       </c>
       <c r="C11" s="0" t="str">
         <f aca="false">CONCATENATE(E11, A11, "_2.fq.gz")</f>
-        <v>/home/cam/test/ndj_08_2.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_08_2.fq.gz</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>18</v>
@@ -805,11 +811,11 @@
       </c>
       <c r="B12" s="0" t="str">
         <f aca="false">CONCATENATE(E12, A12, "_1.fq.gz")</f>
-        <v>/home/cam/test/ndj_09_1.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_09_1.fq.gz</v>
       </c>
       <c r="C12" s="0" t="str">
         <f aca="false">CONCATENATE(E12, A12, "_2.fq.gz")</f>
-        <v>/home/cam/test/ndj_09_2.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_09_2.fq.gz</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>18</v>
@@ -824,11 +830,11 @@
       </c>
       <c r="B13" s="0" t="str">
         <f aca="false">CONCATENATE(E13, A13, "_1.fq.gz")</f>
-        <v>/home/cam/test/ndj_10_1.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_10_1.fq.gz</v>
       </c>
       <c r="C13" s="0" t="str">
         <f aca="false">CONCATENATE(E13, A13, "_2.fq.gz")</f>
-        <v>/home/cam/test/ndj_10_2.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_10_2.fq.gz</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>18</v>
@@ -843,11 +849,11 @@
       </c>
       <c r="B14" s="0" t="str">
         <f aca="false">CONCATENATE(E14, A14, "_1.fq.gz")</f>
-        <v>/home/cam/test/ndj_11_1.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_11_1.fq.gz</v>
       </c>
       <c r="C14" s="0" t="str">
         <f aca="false">CONCATENATE(E14, A14, "_2.fq.gz")</f>
-        <v>/home/cam/test/ndj_11_2.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_11_2.fq.gz</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>18</v>
@@ -862,11 +868,11 @@
       </c>
       <c r="B15" s="0" t="str">
         <f aca="false">CONCATENATE(E15, A15, "_1.fq.gz")</f>
-        <v>/home/cam/test/ndj_12_1.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_12_1.fq.gz</v>
       </c>
       <c r="C15" s="0" t="str">
         <f aca="false">CONCATENATE(E15, A15, "_2.fq.gz")</f>
-        <v>/home/cam/test/ndj_12_2.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_12_2.fq.gz</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>18</v>
@@ -881,11 +887,11 @@
       </c>
       <c r="B16" s="0" t="str">
         <f aca="false">CONCATENATE(E16, A16, "_1.fq.gz")</f>
-        <v>/home/cam/test/ndj_13_1.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_13_1.fq.gz</v>
       </c>
       <c r="C16" s="0" t="str">
         <f aca="false">CONCATENATE(E16, A16, "_2.fq.gz")</f>
-        <v>/home/cam/test/ndj_13_2.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_13_2.fq.gz</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>18</v>
@@ -900,11 +906,11 @@
       </c>
       <c r="B17" s="0" t="str">
         <f aca="false">CONCATENATE(E17, A17, "_1.fq.gz")</f>
-        <v>/home/cam/test/ndj_14_1.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_14_1.fq.gz</v>
       </c>
       <c r="C17" s="0" t="str">
         <f aca="false">CONCATENATE(E17, A17, "_2.fq.gz")</f>
-        <v>/home/cam/test/ndj_14_2.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_14_2.fq.gz</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>18</v>
@@ -919,11 +925,11 @@
       </c>
       <c r="B18" s="0" t="str">
         <f aca="false">CONCATENATE(E18, A18, "_1.fq.gz")</f>
-        <v>/home/cam/test/ndj_15_1.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_15_1.fq.gz</v>
       </c>
       <c r="C18" s="0" t="str">
         <f aca="false">CONCATENATE(E18, A18, "_2.fq.gz")</f>
-        <v>/home/cam/test/ndj_15_2.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_15_2.fq.gz</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>18</v>
@@ -938,16 +944,35 @@
       </c>
       <c r="B19" s="0" t="str">
         <f aca="false">CONCATENATE(E19, A19, "_1.fq.gz")</f>
-        <v>/home/cam/test/ndj_16_1.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_16_1.fq.gz</v>
       </c>
       <c r="C19" s="0" t="str">
         <f aca="false">CONCATENATE(E19, A19, "_2.fq.gz")</f>
-        <v>/home/cam/test/ndj_16_2.fq.gz</v>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/ndj_16_2.fq.gz</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E19" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="0" t="str">
+        <f aca="false">CONCATENATE(E20, A20, "_1.fq.gz")</f>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/hetsub_1.fq.gz</v>
+      </c>
+      <c r="C20" s="0" t="str">
+        <f aca="false">CONCATENATE(E20, A20, "_2.fq.gz")</f>
+        <v>/work/users/c/a/cannecar/ndj_project/reads/hetsub_2.fq.gz</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="0" t="s">
         <v>26</v>
       </c>
     </row>
@@ -973,7 +998,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.95"/>
@@ -985,7 +1010,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>11</v>
@@ -1006,7 +1031,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1021,7 +1046,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1036,7 +1061,7 @@
         <v>18</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1051,7 +1076,7 @@
         <v>18</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1066,7 +1091,7 @@
         <v>18</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1081,7 +1106,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1096,7 +1121,7 @@
         <v>18</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1111,7 +1136,7 @@
         <v>18</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1126,7 +1151,7 @@
         <v>18</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1141,7 +1166,7 @@
         <v>18</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1156,7 +1181,7 @@
         <v>18</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1171,7 +1196,7 @@
         <v>18</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1186,7 +1211,7 @@
         <v>18</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1201,7 +1226,7 @@
         <v>18</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1216,7 +1241,7 @@
         <v>18</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1231,7 +1256,7 @@
         <v>18</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1246,7 +1271,7 @@
         <v>18</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1261,7 +1286,7 @@
         <v>18</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
functional for ndj analysis with bcftools single calling
</commit_message>
<xml_diff>
--- a/sample_sheet.xlsx
+++ b/sample_sheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="48">
   <si>
     <t xml:space="preserve">INSTRUCTIONS</t>
   </si>
@@ -102,7 +102,22 @@
     <t xml:space="preserve">path_to_reads_2</t>
   </si>
   <si>
+    <t xml:space="preserve">trim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read_1_adapter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read_2_adapter</t>
+  </si>
+  <si>
     <t xml:space="preserve">/work/users/c/a/cannecar/ndj_project/reads/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGATCGGAAGAGCGTCGTGTAGGGAAAGAGTGTAGATCTCGGTGGTCGCCGTATCATT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GATCGGAAGAGCACACGTCTGAACTCCAGTCACGGATGACTATCTCGTATGCCGTCTTCTGCTTG</t>
   </si>
   <si>
     <t xml:space="preserve">ndj_04</t>
@@ -157,8 +172,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -232,7 +248,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -246,6 +262,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -272,11 +292,10 @@
       <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="72.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="40.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="29.08"/>
   </cols>
   <sheetData>
@@ -583,17 +602,19 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="94.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="74.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="81.88"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,7 +633,15 @@
       <c r="E1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="0"/>
+      <c r="F1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="K1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -631,7 +660,10 @@
         <v>14</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="F2" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -650,7 +682,10 @@
         <v>14</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="F3" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -669,7 +704,16 @@
         <v>18</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="F4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -688,7 +732,16 @@
         <v>18</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="F5" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -707,12 +760,21 @@
         <v>18</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="F6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B7" s="0" t="str">
         <f aca="false">CONCATENATE(E7, A7, "_1.fq.gz")</f>
@@ -726,12 +788,21 @@
         <v>18</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="F7" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B8" s="0" t="str">
         <f aca="false">CONCATENATE(E8, A8, "_1.fq.gz")</f>
@@ -745,12 +816,21 @@
         <v>18</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="F8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B9" s="0" t="str">
         <f aca="false">CONCATENATE(E9, A9, "_1.fq.gz")</f>
@@ -764,12 +844,21 @@
         <v>18</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="F9" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B10" s="0" t="str">
         <f aca="false">CONCATENATE(E10, A10, "_1.fq.gz")</f>
@@ -783,12 +872,21 @@
         <v>18</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="F10" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B11" s="0" t="str">
         <f aca="false">CONCATENATE(E11, A11, "_1.fq.gz")</f>
@@ -802,12 +900,21 @@
         <v>18</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="F11" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B12" s="0" t="str">
         <f aca="false">CONCATENATE(E12, A12, "_1.fq.gz")</f>
@@ -821,12 +928,21 @@
         <v>18</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="F12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B13" s="0" t="str">
         <f aca="false">CONCATENATE(E13, A13, "_1.fq.gz")</f>
@@ -840,12 +956,21 @@
         <v>18</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="F13" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B14" s="0" t="str">
         <f aca="false">CONCATENATE(E14, A14, "_1.fq.gz")</f>
@@ -859,12 +984,21 @@
         <v>18</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="F14" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B15" s="0" t="str">
         <f aca="false">CONCATENATE(E15, A15, "_1.fq.gz")</f>
@@ -878,12 +1012,21 @@
         <v>18</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="F15" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B16" s="0" t="str">
         <f aca="false">CONCATENATE(E16, A16, "_1.fq.gz")</f>
@@ -897,12 +1040,21 @@
         <v>18</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="F16" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B17" s="0" t="str">
         <f aca="false">CONCATENATE(E17, A17, "_1.fq.gz")</f>
@@ -916,12 +1068,21 @@
         <v>18</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="F17" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B18" s="0" t="str">
         <f aca="false">CONCATENATE(E18, A18, "_1.fq.gz")</f>
@@ -935,12 +1096,21 @@
         <v>18</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="F18" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B19" s="0" t="str">
         <f aca="false">CONCATENATE(E19, A19, "_1.fq.gz")</f>
@@ -954,12 +1124,21 @@
         <v>18</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="F19" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B20" s="0" t="str">
         <f aca="false">CONCATENATE(E20, A20, "_1.fq.gz")</f>
@@ -973,7 +1152,10 @@
         <v>18</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="F20" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -998,7 +1180,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.95"/>
@@ -1010,7 +1192,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>11</v>
@@ -1031,7 +1213,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1046,7 +1228,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1061,7 +1243,7 @@
         <v>18</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,7 +1258,7 @@
         <v>18</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1091,12 +1273,12 @@
         <v>18</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B7" s="0" t="str">
         <f aca="false">CONCATENATE(D7, A7, ".fq.gz")</f>
@@ -1106,12 +1288,12 @@
         <v>18</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B8" s="0" t="str">
         <f aca="false">CONCATENATE(D8, A8, ".fq.gz")</f>
@@ -1121,12 +1303,12 @@
         <v>18</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B9" s="0" t="str">
         <f aca="false">CONCATENATE(D9, A9, ".fq.gz")</f>
@@ -1136,12 +1318,12 @@
         <v>18</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B10" s="0" t="str">
         <f aca="false">CONCATENATE(D10, A10, ".fq.gz")</f>
@@ -1151,12 +1333,12 @@
         <v>18</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B11" s="0" t="str">
         <f aca="false">CONCATENATE(D11, A11, ".fq.gz")</f>
@@ -1166,12 +1348,12 @@
         <v>18</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B12" s="0" t="str">
         <f aca="false">CONCATENATE(D12, A12, ".fq.gz")</f>
@@ -1181,12 +1363,12 @@
         <v>18</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B13" s="0" t="str">
         <f aca="false">CONCATENATE(D13, A13, ".fq.gz")</f>
@@ -1196,12 +1378,12 @@
         <v>18</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B14" s="0" t="str">
         <f aca="false">CONCATENATE(D14, A14, ".fq.gz")</f>
@@ -1211,12 +1393,12 @@
         <v>18</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B15" s="0" t="str">
         <f aca="false">CONCATENATE(D15, A15, ".fq.gz")</f>
@@ -1226,12 +1408,12 @@
         <v>18</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B16" s="0" t="str">
         <f aca="false">CONCATENATE(D16, A16, ".fq.gz")</f>
@@ -1241,12 +1423,12 @@
         <v>18</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B17" s="0" t="str">
         <f aca="false">CONCATENATE(D17, A17, ".fq.gz")</f>
@@ -1256,12 +1438,12 @@
         <v>18</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B18" s="0" t="str">
         <f aca="false">CONCATENATE(D18, A18, ".fq.gz")</f>
@@ -1271,12 +1453,12 @@
         <v>18</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B19" s="0" t="str">
         <f aca="false">CONCATENATE(D19, A19, ".fq.gz")</f>
@@ -1286,7 +1468,7 @@
         <v>18</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>